<commit_message>
Revision estimacion de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Ventas/Estimacion.xlsx
+++ b/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Ventas/Estimacion.xlsx
@@ -142,19 +142,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="102.49887640449438"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.19887640449438"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.99887640449438"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.098876404494384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
         <is>
-          <t>Administración de costos del proyecto "nombre de proyecto"</t>
+          <t>Administración de costos del proyecto</t>
         </is>
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>Administrador de proyecto:   Fecha: </t>
+          <t>Costos de proyecto</t>
         </is>
       </c>
     </row>
@@ -238,7 +238,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1236,138 +1236,6 @@
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="inlineStr">
-        <is>
-          <t>Control de cambios</t>
-        </is>
-      </c>
-      <c r="B32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G32" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="inlineStr">
-        <is>
-          <t>Recibir y Generar solicitud de cambios</t>
-        </is>
-      </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="E33" s="3" t="str">
-        <f>SUM(C33)*SUM(D33)</f>
-      </c>
-      <c r="F33" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G33" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="inlineStr">
-        <is>
-          <t>Analizar solicitud de cambios</t>
-        </is>
-      </c>
-      <c r="B34" s="3" t="inlineStr">
-        <is>
-          <t>CCC</t>
-        </is>
-      </c>
-      <c r="C34" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="E34" s="3" t="str">
-        <f>SUM(C34)*SUM(D34)</f>
-      </c>
-      <c r="F34" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G34" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="inlineStr">
-        <is>
-          <t>Notificar cambios y actualizar documentos</t>
-        </is>
-      </c>
-      <c r="B35" s="3" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="C35" s="3" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E35" s="3" t="str">
-        <f>SUM(C35)*SUM(D35)</f>
-      </c>
-      <c r="F35" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="G35" s="3" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>